<commit_message>
Baguette eating...updated data through 3/31
</commit_message>
<xml_diff>
--- a/librelink/Librelink.xlsx
+++ b/librelink/Librelink.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8bc6084b92ffa451/Sprague 2019/Health 2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{1DF15EB1-8D61-6642-9AC4-0A049F576367}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{3A491F5F-A3B3-644E-8D42-249D0332B2F0}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="13_ncr:1_{1DF15EB1-8D61-6642-9AC4-0A049F576367}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{55C9846D-999F-2240-A4EF-0F4E8FA43194}"/>
   <bookViews>
-    <workbookView xWindow="13960" yWindow="1700" windowWidth="17400" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13920" yWindow="1180" windowWidth="17400" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Librelink" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="66">
   <si>
     <t>Meter</t>
   </si>
@@ -220,6 +220,12 @@
   </si>
   <si>
     <t>Pizza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baguette </t>
+  </si>
+  <si>
+    <t>Burger</t>
   </si>
 </sst>
 </file>
@@ -785,8 +791,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF602BB5-9469-1B45-BB1A-DFBEABAFCD1B}" name="Table1" displayName="Table1" ref="A1:S3964" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:S3964" xr:uid="{A8E95FAB-7D33-F24D-8350-CC174D759A60}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF602BB5-9469-1B45-BB1A-DFBEABAFCD1B}" name="Table1" displayName="Table1" ref="A1:S4083" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:S4083" xr:uid="{A8E95FAB-7D33-F24D-8350-CC174D759A60}"/>
   <tableColumns count="19">
     <tableColumn id="1" xr3:uid="{374D21D6-0283-C44B-8028-4060CB201675}" name="Meter"/>
     <tableColumn id="2" xr3:uid="{48610F22-94E8-1142-AF15-100D6756BE81}" name="Serial Number"/>
@@ -1109,12 +1115,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S3964"/>
+  <dimension ref="A1:S4083"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3836" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A4001" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="C3864" sqref="C3864:H3964"/>
+      <selection pane="bottomLeft" activeCell="C4018" sqref="C4018"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -46360,6 +46366,1315 @@
         <v>87</v>
       </c>
     </row>
+    <row r="3965" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C3965" s="1">
+        <v>43555.318055555559</v>
+      </c>
+      <c r="D3965">
+        <v>0</v>
+      </c>
+      <c r="E3965">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3966" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C3966" s="1">
+        <v>43555.328472222223</v>
+      </c>
+      <c r="D3966">
+        <v>0</v>
+      </c>
+      <c r="E3966">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3967" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C3967" s="1">
+        <v>43555.331944444442</v>
+      </c>
+      <c r="D3967">
+        <v>1</v>
+      </c>
+      <c r="F3967">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3968" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C3968" s="1">
+        <v>43555.338888888888</v>
+      </c>
+      <c r="D3968">
+        <v>0</v>
+      </c>
+      <c r="E3968">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3969" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C3969" s="1">
+        <v>43555.349305555559</v>
+      </c>
+      <c r="D3969">
+        <v>0</v>
+      </c>
+      <c r="E3969">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3970" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C3970" s="1">
+        <v>43555.354861111111</v>
+      </c>
+      <c r="D3970">
+        <v>1</v>
+      </c>
+      <c r="F3970">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3971" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C3971" s="1">
+        <v>43555.36041666667</v>
+      </c>
+      <c r="D3971">
+        <v>0</v>
+      </c>
+      <c r="E3971">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3972" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C3972" s="1">
+        <v>43555.368750000001</v>
+      </c>
+      <c r="D3972">
+        <v>1</v>
+      </c>
+      <c r="F3972">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3973" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C3973" s="1">
+        <v>43555.370833333334</v>
+      </c>
+      <c r="D3973">
+        <v>0</v>
+      </c>
+      <c r="E3973">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3974" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C3974" s="1">
+        <v>43555.381249999999</v>
+      </c>
+      <c r="D3974">
+        <v>0</v>
+      </c>
+      <c r="E3974">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3975" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C3975" s="1">
+        <v>43555.39166666667</v>
+      </c>
+      <c r="D3975">
+        <v>0</v>
+      </c>
+      <c r="E3975">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3976" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C3976" s="1">
+        <v>43555.402083333334</v>
+      </c>
+      <c r="D3976">
+        <v>0</v>
+      </c>
+      <c r="E3976">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3977" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C3977" s="1">
+        <v>43555.412499999999</v>
+      </c>
+      <c r="D3977">
+        <v>0</v>
+      </c>
+      <c r="E3977">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3978" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C3978" s="1">
+        <v>43555.423611111109</v>
+      </c>
+      <c r="D3978">
+        <v>0</v>
+      </c>
+      <c r="E3978">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3979" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C3979" s="1">
+        <v>43555.423611111109</v>
+      </c>
+      <c r="D3979">
+        <v>1</v>
+      </c>
+      <c r="F3979">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3980" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C3980" s="1">
+        <v>43555.434027777781</v>
+      </c>
+      <c r="D3980">
+        <v>0</v>
+      </c>
+      <c r="E3980">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3981" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C3981" s="1">
+        <v>43555.444444444445</v>
+      </c>
+      <c r="D3981">
+        <v>0</v>
+      </c>
+      <c r="E3981">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3982" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C3982" s="1">
+        <v>43555.454861111109</v>
+      </c>
+      <c r="D3982">
+        <v>0</v>
+      </c>
+      <c r="E3982">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3983" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C3983" s="1">
+        <v>43555.456250000003</v>
+      </c>
+      <c r="D3983">
+        <v>1</v>
+      </c>
+      <c r="F3983">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3984" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C3984" s="1">
+        <v>43555.456250000003</v>
+      </c>
+      <c r="D3984">
+        <v>6</v>
+      </c>
+      <c r="N3984" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3985" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C3985" s="1">
+        <v>43555.465277777781</v>
+      </c>
+      <c r="D3985">
+        <v>0</v>
+      </c>
+      <c r="E3985">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3986" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C3986" s="1">
+        <v>43555.46875</v>
+      </c>
+      <c r="D3986">
+        <v>1</v>
+      </c>
+      <c r="F3986">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3987" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C3987" s="1">
+        <v>43555.469444444447</v>
+      </c>
+      <c r="D3987">
+        <v>1</v>
+      </c>
+      <c r="F3987">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3988" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C3988" s="1">
+        <v>43555.475694444445</v>
+      </c>
+      <c r="D3988">
+        <v>0</v>
+      </c>
+      <c r="E3988">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3989" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C3989" s="1">
+        <v>43555.486111111109</v>
+      </c>
+      <c r="D3989">
+        <v>0</v>
+      </c>
+      <c r="E3989">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3990" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C3990" s="1">
+        <v>43555.486805555556</v>
+      </c>
+      <c r="D3990">
+        <v>1</v>
+      </c>
+      <c r="F3990">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3991" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C3991" s="1">
+        <v>43555.489583333336</v>
+      </c>
+      <c r="D3991">
+        <v>1</v>
+      </c>
+      <c r="F3991">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3992" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C3992" s="1">
+        <v>43555.493055555555</v>
+      </c>
+      <c r="D3992">
+        <v>1</v>
+      </c>
+      <c r="F3992">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3993" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C3993" s="1">
+        <v>43555.496527777781</v>
+      </c>
+      <c r="D3993">
+        <v>0</v>
+      </c>
+      <c r="E3993">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3994" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C3994" s="1">
+        <v>43555.498611111114</v>
+      </c>
+      <c r="D3994">
+        <v>1</v>
+      </c>
+      <c r="F3994">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3995" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C3995" s="1">
+        <v>43555.5</v>
+      </c>
+      <c r="D3995">
+        <v>1</v>
+      </c>
+      <c r="F3995">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3996" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C3996" s="1">
+        <v>43555.503472222219</v>
+      </c>
+      <c r="D3996">
+        <v>1</v>
+      </c>
+      <c r="F3996">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3997" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C3997" s="1">
+        <v>43555.506944444445</v>
+      </c>
+      <c r="D3997">
+        <v>1</v>
+      </c>
+      <c r="F3997">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3998" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C3998" s="1">
+        <v>43555.506944444445</v>
+      </c>
+      <c r="D3998">
+        <v>6</v>
+      </c>
+      <c r="N3998" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3999" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C3999" s="1">
+        <v>43555.507638888892</v>
+      </c>
+      <c r="D3999">
+        <v>0</v>
+      </c>
+      <c r="E3999">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4000" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4000" s="1">
+        <v>43555.510416666664</v>
+      </c>
+      <c r="D4000">
+        <v>1</v>
+      </c>
+      <c r="F4000">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4001" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4001" s="1">
+        <v>43555.513888888891</v>
+      </c>
+      <c r="D4001">
+        <v>1</v>
+      </c>
+      <c r="F4001">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4002" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4002" s="1">
+        <v>43555.518055555556</v>
+      </c>
+      <c r="D4002">
+        <v>0</v>
+      </c>
+      <c r="E4002">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4003" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4003" s="1">
+        <v>43555.52847222222</v>
+      </c>
+      <c r="D4003">
+        <v>0</v>
+      </c>
+      <c r="E4003">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4004" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4004" s="1">
+        <v>43555.538888888892</v>
+      </c>
+      <c r="D4004">
+        <v>0</v>
+      </c>
+      <c r="E4004">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4005" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4005" s="1">
+        <v>43555.549305555556</v>
+      </c>
+      <c r="D4005">
+        <v>0</v>
+      </c>
+      <c r="E4005">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4006" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4006" s="1">
+        <v>43555.55972222222</v>
+      </c>
+      <c r="D4006">
+        <v>0</v>
+      </c>
+      <c r="E4006">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4007" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4007" s="1">
+        <v>43555.570138888892</v>
+      </c>
+      <c r="D4007">
+        <v>0</v>
+      </c>
+      <c r="E4007">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4008" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4008" s="1">
+        <v>43555.581250000003</v>
+      </c>
+      <c r="D4008">
+        <v>0</v>
+      </c>
+      <c r="E4008">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4009" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4009" s="1">
+        <v>43555.586805555555</v>
+      </c>
+      <c r="D4009">
+        <v>1</v>
+      </c>
+      <c r="F4009">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4010" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4010" s="1">
+        <v>43555.591666666667</v>
+      </c>
+      <c r="D4010">
+        <v>0</v>
+      </c>
+      <c r="E4010">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4011" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4011" s="1">
+        <v>43555.602083333331</v>
+      </c>
+      <c r="D4011">
+        <v>0</v>
+      </c>
+      <c r="E4011">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4012" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4012" s="1">
+        <v>43555.60833333333</v>
+      </c>
+      <c r="D4012">
+        <v>1</v>
+      </c>
+      <c r="F4012">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4013" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4013" s="1">
+        <v>43555.612500000003</v>
+      </c>
+      <c r="D4013">
+        <v>0</v>
+      </c>
+      <c r="E4013">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4014" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4014" s="1">
+        <v>43555.622916666667</v>
+      </c>
+      <c r="D4014">
+        <v>0</v>
+      </c>
+      <c r="E4014">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4015" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4015" s="1">
+        <v>43555.633333333331</v>
+      </c>
+      <c r="D4015">
+        <v>0</v>
+      </c>
+      <c r="E4015">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4016" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4016" s="1">
+        <v>43555.643750000003</v>
+      </c>
+      <c r="D4016">
+        <v>0</v>
+      </c>
+      <c r="E4016">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4017" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4017" s="1">
+        <v>43555.654166666667</v>
+      </c>
+      <c r="D4017">
+        <v>0</v>
+      </c>
+      <c r="E4017">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4018" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4018" s="1">
+        <v>43555.665277777778</v>
+      </c>
+      <c r="D4018">
+        <v>0</v>
+      </c>
+      <c r="E4018">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4019" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4019" s="1">
+        <v>43555.67291666667</v>
+      </c>
+      <c r="D4019">
+        <v>1</v>
+      </c>
+      <c r="F4019">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4020" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4020" s="1">
+        <v>43555.675694444442</v>
+      </c>
+      <c r="D4020">
+        <v>0</v>
+      </c>
+      <c r="E4020">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4021" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4021" s="1">
+        <v>43555.686111111114</v>
+      </c>
+      <c r="D4021">
+        <v>0</v>
+      </c>
+      <c r="E4021">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4022" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4022" s="1">
+        <v>43555.696527777778</v>
+      </c>
+      <c r="D4022">
+        <v>0</v>
+      </c>
+      <c r="E4022">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4023" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4023" s="1">
+        <v>43555.706944444442</v>
+      </c>
+      <c r="D4023">
+        <v>0</v>
+      </c>
+      <c r="E4023">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4024" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4024" s="1">
+        <v>43555.717361111114</v>
+      </c>
+      <c r="D4024">
+        <v>0</v>
+      </c>
+      <c r="E4024">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4025" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4025" s="1">
+        <v>43555.73541666667</v>
+      </c>
+      <c r="D4025">
+        <v>1</v>
+      </c>
+      <c r="F4025">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4026" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4026" s="1">
+        <v>43555.738888888889</v>
+      </c>
+      <c r="D4026">
+        <v>0</v>
+      </c>
+      <c r="E4026">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4027" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4027" s="1">
+        <v>43555.749305555553</v>
+      </c>
+      <c r="D4027">
+        <v>0</v>
+      </c>
+      <c r="E4027">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4028" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4028" s="1">
+        <v>43555.759722222225</v>
+      </c>
+      <c r="D4028">
+        <v>0</v>
+      </c>
+      <c r="E4028">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4029" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4029" s="1">
+        <v>43555.770138888889</v>
+      </c>
+      <c r="D4029">
+        <v>0</v>
+      </c>
+      <c r="E4029">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4030" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4030" s="1">
+        <v>43555.780555555553</v>
+      </c>
+      <c r="D4030">
+        <v>0</v>
+      </c>
+      <c r="E4030">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4031" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4031" s="1">
+        <v>43555.790972222225</v>
+      </c>
+      <c r="D4031">
+        <v>0</v>
+      </c>
+      <c r="E4031">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4032" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4032" s="1">
+        <v>43555.791666666664</v>
+      </c>
+      <c r="D4032">
+        <v>1</v>
+      </c>
+      <c r="F4032">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4033" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4033" s="1">
+        <v>43555.801388888889</v>
+      </c>
+      <c r="D4033">
+        <v>0</v>
+      </c>
+      <c r="E4033">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4034" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4034" s="1">
+        <v>43555.806944444441</v>
+      </c>
+      <c r="D4034">
+        <v>1</v>
+      </c>
+      <c r="F4034">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4035" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4035" s="1">
+        <v>43555.8125</v>
+      </c>
+      <c r="D4035">
+        <v>0</v>
+      </c>
+      <c r="E4035">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4036" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4036" s="1">
+        <v>43555.816666666666</v>
+      </c>
+      <c r="D4036">
+        <v>1</v>
+      </c>
+      <c r="F4036">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4037" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4037" s="1">
+        <v>43555.822916666664</v>
+      </c>
+      <c r="D4037">
+        <v>0</v>
+      </c>
+      <c r="E4037">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4038" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4038" s="1">
+        <v>43555.833333333336</v>
+      </c>
+      <c r="D4038">
+        <v>0</v>
+      </c>
+      <c r="E4038">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4039" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4039" s="1">
+        <v>43555.84375</v>
+      </c>
+      <c r="D4039">
+        <v>0</v>
+      </c>
+      <c r="E4039">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4040" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4040" s="1">
+        <v>43555.854166666664</v>
+      </c>
+      <c r="D4040">
+        <v>0</v>
+      </c>
+      <c r="E4040">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4041" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4041" s="1">
+        <v>43555.864583333336</v>
+      </c>
+      <c r="D4041">
+        <v>0</v>
+      </c>
+      <c r="E4041">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4042" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4042" s="1">
+        <v>43555.875</v>
+      </c>
+      <c r="D4042">
+        <v>0</v>
+      </c>
+      <c r="E4042">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4043" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4043" s="1">
+        <v>43555.885416666664</v>
+      </c>
+      <c r="D4043">
+        <v>0</v>
+      </c>
+      <c r="E4043">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4044" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4044" s="1">
+        <v>43555.89166666667</v>
+      </c>
+      <c r="D4044">
+        <v>1</v>
+      </c>
+      <c r="F4044">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4045" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4045" s="1">
+        <v>43555.895833333336</v>
+      </c>
+      <c r="D4045">
+        <v>0</v>
+      </c>
+      <c r="E4045">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4046" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4046" s="1">
+        <v>43555.90902777778</v>
+      </c>
+      <c r="D4046">
+        <v>1</v>
+      </c>
+      <c r="F4046">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4047" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4047" s="1">
+        <v>43555.931250000001</v>
+      </c>
+      <c r="D4047">
+        <v>0</v>
+      </c>
+      <c r="E4047">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4048" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4048" s="1">
+        <v>43555.941666666666</v>
+      </c>
+      <c r="D4048">
+        <v>0</v>
+      </c>
+      <c r="E4048">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4049" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4049" s="1">
+        <v>43555.95208333333</v>
+      </c>
+      <c r="D4049">
+        <v>0</v>
+      </c>
+      <c r="E4049">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4050" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4050" s="1">
+        <v>43555.962500000001</v>
+      </c>
+      <c r="D4050">
+        <v>0</v>
+      </c>
+      <c r="E4050">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4051" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4051" s="1">
+        <v>43555.972916666666</v>
+      </c>
+      <c r="D4051">
+        <v>0</v>
+      </c>
+      <c r="E4051">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4052" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4052" s="1">
+        <v>43555.98333333333</v>
+      </c>
+      <c r="D4052">
+        <v>0</v>
+      </c>
+      <c r="E4052">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4053" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4053" s="1">
+        <v>43555.993750000001</v>
+      </c>
+      <c r="D4053">
+        <v>0</v>
+      </c>
+      <c r="E4053">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4054" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4054" s="1">
+        <v>43556.004166666666</v>
+      </c>
+      <c r="D4054">
+        <v>0</v>
+      </c>
+      <c r="E4054">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4055" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4055" s="1">
+        <v>43556.01458333333</v>
+      </c>
+      <c r="D4055">
+        <v>0</v>
+      </c>
+      <c r="E4055">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4056" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4056" s="1">
+        <v>43556.025000000001</v>
+      </c>
+      <c r="D4056">
+        <v>0</v>
+      </c>
+      <c r="E4056">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4057" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4057" s="1">
+        <v>43556.035416666666</v>
+      </c>
+      <c r="D4057">
+        <v>0</v>
+      </c>
+      <c r="E4057">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4058" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4058" s="1">
+        <v>43556.04583333333</v>
+      </c>
+      <c r="D4058">
+        <v>0</v>
+      </c>
+      <c r="E4058">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4059" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4059" s="1">
+        <v>43556.056250000001</v>
+      </c>
+      <c r="D4059">
+        <v>0</v>
+      </c>
+      <c r="E4059">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4060" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4060" s="1">
+        <v>43556.066666666666</v>
+      </c>
+      <c r="D4060">
+        <v>0</v>
+      </c>
+      <c r="E4060">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4061" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4061" s="1">
+        <v>43556.07708333333</v>
+      </c>
+      <c r="D4061">
+        <v>0</v>
+      </c>
+      <c r="E4061">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4062" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4062" s="1">
+        <v>43556.087500000001</v>
+      </c>
+      <c r="D4062">
+        <v>0</v>
+      </c>
+      <c r="E4062">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4063" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4063" s="1">
+        <v>43556.097916666666</v>
+      </c>
+      <c r="D4063">
+        <v>0</v>
+      </c>
+      <c r="E4063">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4064" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4064" s="1">
+        <v>43556.10833333333</v>
+      </c>
+      <c r="D4064">
+        <v>0</v>
+      </c>
+      <c r="E4064">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4065" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4065" s="1">
+        <v>43556.118750000001</v>
+      </c>
+      <c r="D4065">
+        <v>0</v>
+      </c>
+      <c r="E4065">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4066" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4066" s="1">
+        <v>43556.129166666666</v>
+      </c>
+      <c r="D4066">
+        <v>0</v>
+      </c>
+      <c r="E4066">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4067" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4067" s="1">
+        <v>43556.13958333333</v>
+      </c>
+      <c r="D4067">
+        <v>0</v>
+      </c>
+      <c r="E4067">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4068" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4068" s="1">
+        <v>43556.15</v>
+      </c>
+      <c r="D4068">
+        <v>0</v>
+      </c>
+      <c r="E4068">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4069" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4069" s="1">
+        <v>43556.160416666666</v>
+      </c>
+      <c r="D4069">
+        <v>0</v>
+      </c>
+      <c r="E4069">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4070" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4070" s="1">
+        <v>43556.17083333333</v>
+      </c>
+      <c r="D4070">
+        <v>0</v>
+      </c>
+      <c r="E4070">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4071" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4071" s="1">
+        <v>43556.181250000001</v>
+      </c>
+      <c r="D4071">
+        <v>0</v>
+      </c>
+      <c r="E4071">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4072" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4072" s="1">
+        <v>43556.191666666666</v>
+      </c>
+      <c r="D4072">
+        <v>0</v>
+      </c>
+      <c r="E4072">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4073" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4073" s="1">
+        <v>43556.20208333333</v>
+      </c>
+      <c r="D4073">
+        <v>0</v>
+      </c>
+      <c r="E4073">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4074" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4074" s="1">
+        <v>43556.212500000001</v>
+      </c>
+      <c r="D4074">
+        <v>0</v>
+      </c>
+      <c r="E4074">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4075" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4075" s="1">
+        <v>43556.222916666666</v>
+      </c>
+      <c r="D4075">
+        <v>0</v>
+      </c>
+      <c r="E4075">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4076" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4076" s="1">
+        <v>43556.23333333333</v>
+      </c>
+      <c r="D4076">
+        <v>0</v>
+      </c>
+      <c r="E4076">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4077" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4077" s="1">
+        <v>43556.243750000001</v>
+      </c>
+      <c r="D4077">
+        <v>0</v>
+      </c>
+      <c r="E4077">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4078" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4078" s="1">
+        <v>43556.254166666666</v>
+      </c>
+      <c r="D4078">
+        <v>0</v>
+      </c>
+      <c r="E4078">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4079" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4079" s="1">
+        <v>43556.261111111111</v>
+      </c>
+      <c r="D4079">
+        <v>1</v>
+      </c>
+      <c r="F4079">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4080" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4080" s="1">
+        <v>43556.26458333333</v>
+      </c>
+      <c r="D4080">
+        <v>0</v>
+      </c>
+      <c r="E4080">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4081" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4081" s="1">
+        <v>43556.275000000001</v>
+      </c>
+      <c r="D4081">
+        <v>0</v>
+      </c>
+      <c r="E4081">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4082" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4082" s="1">
+        <v>43556.283333333333</v>
+      </c>
+      <c r="D4082">
+        <v>1</v>
+      </c>
+      <c r="F4082">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4083" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4083" s="1">
+        <v>43556.287499999999</v>
+      </c>
+      <c r="D4083">
+        <v>1</v>
+      </c>
+      <c r="F4083">
+        <v>83</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">

</xml_diff>